<commit_message>
esercizio 3 modulo 3
</commit_message>
<xml_diff>
--- a/Modulo 3/Progetto_logico.xlsx
+++ b/Modulo 3/Progetto_logico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emanuele\OneDrive\Desktop\Epicode Exercise\Modulo 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CBDCBBB-D527-4B20-9C77-D35ACF69FFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E035DC00-A012-4976-AC2C-7360F4B67277}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{685199E9-AD46-4BD0-AFBE-D9DB3D198C10}"/>
+    <workbookView minimized="1" xWindow="18495" yWindow="2865" windowWidth="10305" windowHeight="12615" activeTab="2" xr2:uid="{685199E9-AD46-4BD0-AFBE-D9DB3D198C10}"/>
   </bookViews>
   <sheets>
     <sheet name="STORE" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>NOME</t>
   </si>
@@ -115,13 +115,16 @@
   </si>
   <si>
     <t>CODICE_FISCALE</t>
+  </si>
+  <si>
+    <t>CARICA_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,21 +162,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <u/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -228,7 +216,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -239,10 +227,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -250,7 +237,7 @@
   <dxfs count="16">
     <dxf>
       <font>
-        <i val="0"/>
+        <i/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -258,62 +245,6 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -341,33 +272,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <strike val="0"/>
@@ -390,24 +294,16 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
-        <u/>
         <vertAlign val="baseline"/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color auto="1"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -432,6 +328,58 @@
     </dxf>
     <dxf>
       <font>
+        <i val="0"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <strike val="0"/>
         <outline val="0"/>
@@ -451,6 +399,46 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -465,40 +453,41 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C949D589-3E37-4132-876F-3C53109DB71A}" name="Tabella2" displayName="Tabella2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C949D589-3E37-4132-876F-3C53109DB71A}" name="Tabella2" displayName="Tabella2" ref="A1:D2" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A1:D2" xr:uid="{C949D589-3E37-4132-876F-3C53109DB71A}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{1227F109-B3DF-4D25-8058-171D92768C8D}" name="ID_STORE" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{1227F109-B3DF-4D25-8058-171D92768C8D}" name="ID_STORE" dataDxfId="14"/>
     <tableColumn id="4" xr3:uid="{472570C5-765B-46ED-B116-90E4F0254C7C}" name="STORE"/>
     <tableColumn id="2" xr3:uid="{19182F0F-544E-49AB-800C-AFF93BF5FC9B}" name="INDIRIZZO"/>
-    <tableColumn id="3" xr3:uid="{38618347-52F2-42B6-95D4-09A6F48BDDD7}" name="TELEFONO" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{38618347-52F2-42B6-95D4-09A6F48BDDD7}" name="TELEFONO" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BD82AC8-19E5-4415-9B1D-40232692C205}" name="Tabella1" displayName="Tabella1" ref="A1:E2" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4BD82AC8-19E5-4415-9B1D-40232692C205}" name="Tabella1" displayName="Tabella1" ref="A1:E2" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A1:E2" xr:uid="{4BD82AC8-19E5-4415-9B1D-40232692C205}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{AEDAE1BE-CB16-4E15-9505-7385B1176756}" name="CODICE_FISCALE" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{3A34AFE0-A9B3-4B7C-97BC-56C61F2B4FD6}" name="NOME" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{6142BF05-52B8-464E-BDB4-201B58206DAF}" name="CARICA" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{CF48CCE7-299E-4F6C-BAB7-21E8CCE035DA}" name="TITOLO_STUDIO" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{E9534EC5-AA9E-4FDD-A1E6-2BD9DA2774AD}" name="RECAPITO" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{AEDAE1BE-CB16-4E15-9505-7385B1176756}" name="CODICE_FISCALE" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{3A34AFE0-A9B3-4B7C-97BC-56C61F2B4FD6}" name="NOME" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{6142BF05-52B8-464E-BDB4-201B58206DAF}" name="CARICA" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{CF48CCE7-299E-4F6C-BAB7-21E8CCE035DA}" name="TITOLO_STUDIO" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{E9534EC5-AA9E-4FDD-A1E6-2BD9DA2774AD}" name="RECAPITO" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F53E6438-64F3-4CC2-B0A7-AA0898E62B5B}" name="Tabella3" displayName="Tabella3" ref="A1:D2" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A1:D2" xr:uid="{F53E6438-64F3-4CC2-B0A7-AA0898E62B5B}"/>
-  <tableColumns count="4">
-    <tableColumn id="4" xr3:uid="{FDF03286-B2D6-42AA-BC3C-F0D32C541BDC}" name="CF_IMPIEGATO" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F53E6438-64F3-4CC2-B0A7-AA0898E62B5B}" name="Tabella3" displayName="Tabella3" ref="A1:E2" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="A1:E2" xr:uid="{F53E6438-64F3-4CC2-B0A7-AA0898E62B5B}"/>
+  <tableColumns count="5">
+    <tableColumn id="4" xr3:uid="{FDF03286-B2D6-42AA-BC3C-F0D32C541BDC}" name="CF_IMPIEGATO" dataDxfId="5"/>
     <tableColumn id="5" xr3:uid="{2015DA7E-E1A9-430B-BF80-8E756E0628A7}" name="DATA_INIZIO"/>
     <tableColumn id="3" xr3:uid="{81960C72-4F03-4260-9165-53D1F3DC2EFA}" name="DATA_FINE"/>
-    <tableColumn id="2" xr3:uid="{8399A59C-13C8-4CB3-9E62-E16A8AC19B1D}" name="CODICE_STORE" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{6B6F450C-3815-42C5-9438-A67E2D2B1E2F}" name="CODICE_STORE"/>
+    <tableColumn id="2" xr3:uid="{8399A59C-13C8-4CB3-9E62-E16A8AC19B1D}" name="CARICA_1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -508,7 +497,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CB2726E5-DD03-42A3-BDC5-5B57A5310F51}" name="Tabella5" displayName="Tabella5" ref="A1:H2" totalsRowShown="0">
   <autoFilter ref="A1:H2" xr:uid="{CB2726E5-DD03-42A3-BDC5-5B57A5310F51}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B7BDB59D-145E-438A-BD11-E5A693FEDA0C}" name="ID_SETTORE" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{B7BDB59D-145E-438A-BD11-E5A693FEDA0C}" name="ID_SETTORE" dataDxfId="4"/>
     <tableColumn id="7" xr3:uid="{683E653F-2AA5-4C7D-9351-23923592042D}" name="TITOLO"/>
     <tableColumn id="9" xr3:uid="{799EEF5B-4183-4CC2-90EE-87B4C8FA41F1}" name="SVILUPPATORE"/>
     <tableColumn id="2" xr3:uid="{BAD67F72-DEAD-40BC-BF1B-3E1948A5275F}" name="N_SETTORE"/>
@@ -522,11 +511,11 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04D93C36-7DE1-4080-B255-A158F4141D89}" name="Tabella6" displayName="Tabella6" ref="A1:F2" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{04D93C36-7DE1-4080-B255-A158F4141D89}" name="Tabella6" displayName="Tabella6" ref="A1:F2" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:F2" xr:uid="{04D93C36-7DE1-4080-B255-A158F4141D89}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{CD66730D-ED4C-4776-9459-6F303B65BE45}" name="TITOLO" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{A29F2D69-60EB-4CBC-9F4D-76DABC504AAF}" name="SVILUPPATORE" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{CD66730D-ED4C-4776-9459-6F303B65BE45}" name="TITOLO" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{A29F2D69-60EB-4CBC-9F4D-76DABC504AAF}" name="SVILUPPATORE" dataDxfId="1"/>
     <tableColumn id="3" xr3:uid="{260F1BD7-193F-4D85-B38F-B26EB8283446}" name="GENERE"/>
     <tableColumn id="4" xr3:uid="{FAD7F0ED-48EB-449F-AABC-4002CFFED6FB}" name="ANNO_DISTRIBUZIONE"/>
     <tableColumn id="5" xr3:uid="{B2408AB9-159F-491B-AF2C-71F64615E761}" name="REMAKE"/>
@@ -914,33 +903,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D420E9-138C-4D59-B2C1-F749B4BA77B7}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>6</v>
       </c>
+      <c r="E1" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E2" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -957,7 +953,7 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -994,7 +990,7 @@
       <c r="G1" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="11" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1010,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD69CAC9-C2E7-42F1-961E-524955548FC5}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>

</xml_diff>